<commit_message>
Demo version for Jan.30
built Jan.27
</commit_message>
<xml_diff>
--- a/site_configurations.xlsx
+++ b/site_configurations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HaZhang\Desktop\clipmaster-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C1467D-43EB-4BCC-B047-81DBA9359282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B55831-CA04-47BE-A073-97BA568659F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="generalRule" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="96">
   <si>
     <t>nytimes.com</t>
   </si>
@@ -239,9 +239,6 @@
     <t>credit,container,text-form-wrapper</t>
   </si>
   <si>
-    <t>syndicated-embedded-player,promo-oneliner newsletter,image-credit</t>
-  </si>
-  <si>
     <t>hatley-campaign Campaign CampaignType--inline,wp-media-credit</t>
   </si>
   <si>
@@ -269,9 +266,6 @@
     <t>BROOKLYN PAPER</t>
   </si>
   <si>
-    <t>wp-caption aligncenter,ad-container embedded-ad-container,promo-oneliner newsletter</t>
-  </si>
-  <si>
     <t>custom,tag-bottom</t>
   </si>
   <si>
@@ -300,6 +294,24 @@
   </si>
   <si>
     <t>css-79elbk,css-1px5j0,related-links-block css-z0eu1t epkadsg3,css-798hid etfikam0,interactive-content interactive-size-scoop css-retkgj,css-1at4x3t,css-f6q96b,css-9tf9ac</t>
+  </si>
+  <si>
+    <t>syndicated-embedded-player,promo-oneliner newsletter,image-credit,wp-caption-text</t>
+  </si>
+  <si>
+    <t>bxtimes.com</t>
+  </si>
+  <si>
+    <t>BRONX TIMES</t>
+  </si>
+  <si>
+    <t>wp-caption aligncenter,ad-container embedded-ad-container,promo-oneliner newsletter,syndicated-embedded-player</t>
+  </si>
+  <si>
+    <t>politico.com</t>
+  </si>
+  <si>
+    <t>em</t>
   </si>
 </sst>
 </file>
@@ -677,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,7 +722,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -752,12 +764,12 @@
         <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>94</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
@@ -766,234 +778,259 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>23</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" t="s">
-        <v>82</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>39</v>
+      </c>
+      <c r="D16" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>54</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B22" t="s">
-        <v>80</v>
-      </c>
-      <c r="C22" t="s">
-        <v>34</v>
-      </c>
       <c r="D22" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" t="s">
         <v>86</v>
       </c>
-      <c r="C23" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
+      <c r="A25" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1142,7 +1179,7 @@
         <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1153,7 +1190,7 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1161,10 +1198,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" t="s">
         <v>87</v>
-      </c>
-      <c r="B10" t="s">
-        <v>89</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1221,9 +1258,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1240,6 +1279,14 @@
         <v>66</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Enable copy to clipboard
minor fixes on opinion detection & chalkbeat rules

Signed-off-by: HWZ <30350209+hanwzhang@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/site_configurations.xlsx
+++ b/site_configurations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HaZhang\Desktop\clipmaster-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B55831-CA04-47BE-A073-97BA568659F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E989232-C780-4F47-B79C-805194574F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="generalRule" sheetId="1" r:id="rId1"/>
@@ -242,9 +242,6 @@
     <t>hatley-campaign Campaign CampaignType--inline,wp-media-credit</t>
   </si>
   <si>
-    <t>Page-articleBody-TagData,GoogleDfpAd-background is_filled</t>
-  </si>
-  <si>
     <t>wp-caption-text,css-1dbjc4n r-13awgt0 r-12vffkv,share-bottom</t>
   </si>
   <si>
@@ -312,6 +309,9 @@
   </si>
   <si>
     <t>em</t>
+  </si>
+  <si>
+    <t>Page-articleBody-TagData,GoogleDfpAd-background is_filled,sponsor-message</t>
   </si>
 </sst>
 </file>
@@ -691,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,7 +722,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -764,12 +764,12 @@
         <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
@@ -778,7 +778,7 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -792,7 +792,7 @@
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -839,7 +839,7 @@
         <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -864,7 +864,7 @@
         <v>31</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -878,7 +878,7 @@
         <v>34</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -903,7 +903,7 @@
         <v>39</v>
       </c>
       <c r="D16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -942,7 +942,7 @@
         <v>31</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -956,7 +956,7 @@
         <v>28</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -970,7 +970,7 @@
         <v>52</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -984,46 +984,46 @@
         <v>55</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" t="s">
         <v>78</v>
-      </c>
-      <c r="B23" t="s">
-        <v>79</v>
       </c>
       <c r="C23" t="s">
         <v>34</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" t="s">
         <v>85</v>
-      </c>
-      <c r="B24" t="s">
-        <v>84</v>
-      </c>
-      <c r="C24" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" t="s">
         <v>91</v>
-      </c>
-      <c r="B25" t="s">
-        <v>92</v>
       </c>
       <c r="C25" t="s">
         <v>34</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1179,7 +1179,7 @@
         <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1190,7 +1190,7 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1198,10 +1198,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1260,8 +1260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,7 +1284,7 @@
         <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix comma issues; new sites
Signed-off-by: HWZ <30350209+hanwzhang@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/site_configurations.xlsx
+++ b/site_configurations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HaZhang\Desktop\clipmaster-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HaZhang\Desktop\clipmaster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E989232-C780-4F47-B79C-805194574F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413D532D-F0D0-4F57-B8A4-986EB080B164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3585" yWindow="2010" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="generalRule" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="104">
   <si>
     <t>nytimes.com</t>
   </si>
@@ -236,9 +236,6 @@
     <t>inline-slideshow,inline-module__inner,social-icons__icon--comments__count,single__inline-module alignleft,comments-inline-cta__wrap,credit</t>
   </si>
   <si>
-    <t>credit,container,text-form-wrapper</t>
-  </si>
-  <si>
     <t>hatley-campaign Campaign CampaignType--inline,wp-media-credit</t>
   </si>
   <si>
@@ -312,6 +309,33 @@
   </si>
   <si>
     <t>Page-articleBody-TagData,GoogleDfpAd-background is_filled,sponsor-message</t>
+  </si>
+  <si>
+    <t>thechiefleader.com</t>
+  </si>
+  <si>
+    <t>CHIEF LEADER</t>
+  </si>
+  <si>
+    <t>body main-body clearfix</t>
+  </si>
+  <si>
+    <t>documentedny.com</t>
+  </si>
+  <si>
+    <t>DOCUMENTED</t>
+  </si>
+  <si>
+    <t>credit,container,text-form-wrapper,newsletter-flex-text</t>
+  </si>
+  <si>
+    <t>row pt-3</t>
+  </si>
+  <si>
+    <t>[class*=light-one-column-row-author-flex]</t>
+  </si>
+  <si>
+    <t>article-div-figure,pt-4 mb-4,main-article-author-div py-2,d-flex flex-wrap main-article-tags-div py-2,sharedaddy sd-sharing-enabled</t>
   </si>
 </sst>
 </file>
@@ -691,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,7 +746,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -750,7 +774,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -764,12 +788,12 @@
         <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
@@ -778,7 +802,7 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -792,7 +816,7 @@
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -839,7 +863,7 @@
         <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -864,7 +888,7 @@
         <v>31</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -878,7 +902,7 @@
         <v>34</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -903,7 +927,7 @@
         <v>39</v>
       </c>
       <c r="D16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -928,7 +952,7 @@
         <v>45</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -942,7 +966,7 @@
         <v>31</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -956,7 +980,7 @@
         <v>28</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -970,7 +994,7 @@
         <v>52</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -984,53 +1008,72 @@
         <v>55</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" t="s">
         <v>77</v>
-      </c>
-      <c r="B23" t="s">
-        <v>78</v>
       </c>
       <c r="C23" t="s">
         <v>34</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" t="s">
         <v>84</v>
-      </c>
-      <c r="B24" t="s">
-        <v>83</v>
-      </c>
-      <c r="C24" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" t="s">
         <v>90</v>
-      </c>
-      <c r="B25" t="s">
-        <v>91</v>
       </c>
       <c r="C25" t="s">
         <v>34</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
+      <c r="A26" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
+      <c r="A27" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" t="s">
+        <v>103</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1092,10 +1135,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,7 +1222,7 @@
         <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1190,7 +1233,7 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1198,12 +1241,23 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11">
         <v>0</v>
       </c>
     </row>
@@ -1214,10 +1268,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,6 +1302,14 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1284,7 +1346,7 @@
         <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove newlines in author
and minor fixes

Signed-off-by: HWZ <30350209+hanwzhang@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/site_configurations.xlsx
+++ b/site_configurations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HaZhang\Desktop\clipmaster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D82DA21-E058-477A-91B2-2AD4AE942AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59571D43-6F76-42F1-BB6B-7062D1EA0C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8085" yWindow="1080" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1095" yWindow="270" windowWidth="14880" windowHeight="14370" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="generalRule" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="109">
   <si>
     <t>nytimes.com</t>
   </si>
@@ -209,9 +209,6 @@
     <t>[class*=byline]</t>
   </si>
   <si>
-    <t>[class*=AuthorByline-InPage]</t>
-  </si>
-  <si>
     <t>[class*=e1jsehar1]</t>
   </si>
   <si>
@@ -251,9 +248,6 @@
     <t>streamfield-paragraph rte-text</t>
   </si>
   <si>
-    <t>ts-share-bar,ad_wrapper,figContainer,interstitial-link block-margin-bottom</t>
-  </si>
-  <si>
     <t>brooklynpaper.com</t>
   </si>
   <si>
@@ -351,6 +345,12 @@
   </si>
   <si>
     <t>wp-caption aligncenter,ad-container embedded-ad-container,promo-oneliner newsletter,syndicated-embedded-player,image-credit, js</t>
+  </si>
+  <si>
+    <t>ts-share-bar,ad_wrapper,figContainer,interstitial-link block-margin-bottom,container-padding container-backgroung container-display-inline-block</t>
+  </si>
+  <si>
+    <t>[class*=Page-authors ]</t>
   </si>
 </sst>
 </file>
@@ -737,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,7 +768,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -782,7 +782,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -796,7 +796,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -810,12 +810,12 @@
         <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
@@ -824,7 +824,7 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -838,7 +838,7 @@
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -874,7 +874,7 @@
         <v>23</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -885,7 +885,7 @@
         <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -910,7 +910,7 @@
         <v>31</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -924,7 +924,7 @@
         <v>34</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -932,7 +932,7 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s">
         <v>36</v>
@@ -949,7 +949,7 @@
         <v>39</v>
       </c>
       <c r="D16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -974,7 +974,7 @@
         <v>45</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -988,7 +988,7 @@
         <v>31</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1002,7 +1002,7 @@
         <v>28</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1016,7 +1016,7 @@
         <v>52</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1030,85 +1030,85 @@
         <v>55</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C23" t="s">
         <v>34</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" t="s">
         <v>82</v>
-      </c>
-      <c r="C24" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C25" t="s">
         <v>34</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" t="s">
         <v>95</v>
-      </c>
-      <c r="B26" t="s">
-        <v>96</v>
-      </c>
-      <c r="C26" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" t="s">
         <v>99</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>101</v>
-      </c>
-      <c r="D27" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B28" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1173,8 +1173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1214,7 +1214,7 @@
         <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1225,7 +1225,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1236,7 +1236,7 @@
         <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1247,7 +1247,7 @@
         <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1258,7 +1258,7 @@
         <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1269,7 +1269,7 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1277,10 +1277,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" t="s">
         <v>83</v>
-      </c>
-      <c r="B10" t="s">
-        <v>85</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1288,10 +1288,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1299,10 +1299,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1318,7 +1318,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1333,7 +1333,7 @@
         <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1341,7 +1341,7 @@
         <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1349,15 +1349,15 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1367,10 +1367,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1385,7 +1385,7 @@
         <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1393,7 +1393,15 @@
         <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>